<commit_message>
Enhance logging in DLLInjector and game_install_controller with improved messages and error handling; implement colored console output for better visibility; update logger setup to create timestamped log files for better tracking of events.
</commit_message>
<xml_diff>
--- a/SteamOKAutomaticScript/result/games.xlsx
+++ b/SteamOKAutomaticScript/result/games.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,19 +459,185 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>En Garde</t>
+          <t>Beyond the Wire</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>是</t>
+          <t>screenshots/Demonologist/detail.png</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Failed to click '马上玩' button</t>
-        </is>
-      </c>
+          <t>Failed to click play button</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Demonologist</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Drug Dealer Simulator 2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>击剑预备！</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Failed to click play button</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Grand Emprise: Time Travel Survival</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Meet Your Maker</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MIR4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Timeout: Failed to stop game or complete installation after 10 attempts</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Omega Strikers</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Timeout: Failed to stop game or complete installation after 10 attempts</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Palia</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Senua’s Saga: Hellblade II</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Superfuse</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>VEILED EXPERTS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update games.xlsx with new game data, reflecting recent changes for improved processing accuracy.
</commit_message>
<xml_diff>
--- a/SteamOKAutomaticScript/result/games.xlsx
+++ b/SteamOKAutomaticScript/result/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>steamid</t>
   </si>
@@ -31,16 +31,13 @@
     <t>Beyond the Wire</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Demonologist</t>
   </si>
   <si>
     <t>Drug Dealer Simulator 2</t>
   </si>
   <si>
-    <t>击剑预备！</t>
+    <t>En Garde!</t>
   </si>
   <si>
     <t>Grand Emprise: Time Travel Survival</t>
@@ -65,9 +62,6 @@
   </si>
   <si>
     <t>VEILED EXPERTS</t>
-  </si>
-  <si>
-    <t>En Garde!</t>
   </si>
   <si>
     <t>Crab Champions</t>
@@ -124,7 +118,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -177,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,16 +179,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -511,13 +502,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,41 +527,29 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -578,7 +557,7 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -586,7 +565,7 @@
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -594,7 +573,7 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -602,7 +581,7 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -610,7 +589,7 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -618,7 +597,7 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -626,7 +605,7 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -634,147 +613,147 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="6">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="6">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="6">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="6">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="6">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="6">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="6">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="6">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>

</xml_diff>